<commit_message>
little catalog changes, small screen adapt
</commit_message>
<xml_diff>
--- a/Articulos.xlsx
+++ b/Articulos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="64">
   <si>
     <t>Tipo</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Artículo</t>
   </si>
   <si>
-    <t>Hecho</t>
-  </si>
-  <si>
     <t>Mangos escurridores</t>
   </si>
   <si>
@@ -213,6 +210,15 @@
   </si>
   <si>
     <t>202-b</t>
+  </si>
+  <si>
+    <t>Los  3 son iguales</t>
+  </si>
+  <si>
+    <t>No hay foto grande</t>
+  </si>
+  <si>
+    <t>no hay foto grande</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,10 +294,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -569,18 +582,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A168" workbookViewId="0">
-      <selection activeCell="D173" sqref="D173"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <f>SUM(A2:A172)</f>
+        <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -589,12 +604,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>5</v>
@@ -602,13 +614,10 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>6</v>
@@ -616,13 +625,10 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>21</v>
@@ -630,13 +636,10 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>22</v>
@@ -645,9 +648,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>46</v>
@@ -656,9 +659,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>47</v>
@@ -667,9 +670,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>48</v>
@@ -678,9 +681,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>49</v>
@@ -689,9 +692,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -700,9 +703,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>51</v>
@@ -711,42 +714,42 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" t="s">
         <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
       </c>
       <c r="D12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
         <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
       </c>
       <c r="D13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>63</v>
@@ -755,9 +758,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>74</v>
@@ -768,7 +771,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>75</v>
@@ -779,7 +782,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>81</v>
@@ -790,7 +793,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>89</v>
@@ -801,7 +804,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>101</v>
@@ -812,10 +815,10 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -823,7 +826,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>102</v>
@@ -834,7 +837,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>121</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>122</v>
@@ -856,7 +859,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>126</v>
@@ -867,7 +870,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>128</v>
@@ -878,7 +881,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C27">
         <v>129</v>
@@ -889,10 +892,10 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D28">
         <v>27</v>
@@ -900,7 +903,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C29">
         <v>157</v>
@@ -911,7 +914,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>158</v>
@@ -922,7 +925,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31">
         <v>163</v>
@@ -933,18 +936,18 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <v>70</v>
@@ -953,9 +956,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>186</v>
@@ -964,9 +967,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35">
         <v>202</v>
@@ -975,64 +978,64 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D37">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D39">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D40">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>207</v>
@@ -1041,9 +1044,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>213</v>
@@ -1052,9 +1055,9 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>221</v>
@@ -1063,9 +1066,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>230</v>
@@ -1074,9 +1077,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C45">
         <v>241</v>
@@ -1085,9 +1088,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>82</v>
@@ -1096,9 +1099,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>12</v>
@@ -1110,12 +1116,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
       <c r="B48" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C48" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>47</v>
@@ -1124,9 +1133,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>45</v>
@@ -1138,12 +1150,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D50">
         <v>49</v>
@@ -1152,12 +1167,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D51">
         <v>50</v>
@@ -1166,9 +1184,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
       <c r="B52" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52">
         <v>65</v>
@@ -1180,12 +1201,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D53">
         <v>52</v>
@@ -1194,9 +1218,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
       <c r="B54" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C54">
         <v>79</v>
@@ -1208,12 +1235,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1</v>
+      </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D55">
         <v>54</v>
@@ -1222,12 +1252,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1</v>
+      </c>
       <c r="B56" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D56">
         <v>55</v>
@@ -1236,12 +1269,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D57">
         <v>56</v>
@@ -1250,9 +1286,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
       <c r="B58" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58">
         <v>146</v>
@@ -1264,9 +1303,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59">
         <v>147</v>
@@ -1278,9 +1320,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
       <c r="B60" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C60">
         <v>148</v>
@@ -1292,9 +1337,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61">
         <v>149</v>
@@ -1306,9 +1354,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
       <c r="B62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <v>152</v>
@@ -1320,12 +1371,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
       <c r="B63" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C63" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D63">
         <v>62</v>
@@ -1334,12 +1388,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D64">
         <v>63</v>
@@ -1348,12 +1405,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
       <c r="B65" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D65">
         <v>64</v>
@@ -1362,12 +1422,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>1</v>
+      </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D66">
         <v>65</v>
@@ -1375,10 +1438,16 @@
       <c r="E66" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F66" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>1</v>
+      </c>
       <c r="B67" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>13</v>
@@ -1390,12 +1459,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>1</v>
+      </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D68">
         <v>67</v>
@@ -1404,12 +1476,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1</v>
+      </c>
       <c r="B69" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D69">
         <v>68</v>
@@ -1418,9 +1493,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1</v>
+      </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C70">
         <v>14</v>
@@ -1432,12 +1510,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1</v>
+      </c>
       <c r="B71" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C71" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D71">
         <v>70</v>
@@ -1446,12 +1527,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>1</v>
+      </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D72">
         <v>71</v>
@@ -1460,12 +1544,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>1</v>
+      </c>
       <c r="B73" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D73">
         <v>72</v>
@@ -1474,12 +1561,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>1</v>
+      </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D74">
         <v>73</v>
@@ -1488,12 +1578,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>1</v>
+      </c>
       <c r="B75" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C75" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D75">
         <v>74</v>
@@ -1502,9 +1595,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>1</v>
+      </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C76">
         <v>19</v>
@@ -1516,9 +1612,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>1</v>
+      </c>
       <c r="B77" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C77">
         <v>26</v>
@@ -1530,9 +1629,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>1</v>
+      </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C78">
         <v>31</v>
@@ -1544,9 +1646,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>1</v>
+      </c>
       <c r="B79" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79">
         <v>32</v>
@@ -1558,9 +1663,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>1</v>
+      </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C80">
         <v>33</v>
@@ -1572,9 +1680,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>1</v>
+      </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C81">
         <v>39</v>
@@ -1586,9 +1697,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>1</v>
+      </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C82">
         <v>64</v>
@@ -1600,9 +1714,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>1</v>
+      </c>
       <c r="B83" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C83">
         <v>70</v>
@@ -1614,9 +1731,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>1</v>
+      </c>
       <c r="B84" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C84">
         <v>71</v>
@@ -1628,9 +1748,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>1</v>
+      </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <v>83</v>
@@ -1642,9 +1765,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>1</v>
+      </c>
       <c r="B86" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C86">
         <v>88</v>
@@ -1656,9 +1782,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>1</v>
+      </c>
       <c r="B87" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <v>97</v>
@@ -1670,9 +1799,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>1</v>
+      </c>
       <c r="B88" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C88">
         <v>98</v>
@@ -1684,9 +1816,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>1</v>
+      </c>
       <c r="B89" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C89">
         <v>99</v>
@@ -1698,9 +1833,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>1</v>
+      </c>
       <c r="B90" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C90">
         <v>103</v>
@@ -1712,9 +1850,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>1</v>
+      </c>
       <c r="B91" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C91">
         <v>104</v>
@@ -1726,9 +1867,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>1</v>
+      </c>
       <c r="B92" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C92">
         <v>105</v>
@@ -1740,9 +1884,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>1</v>
+      </c>
       <c r="B93" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93">
         <v>110</v>
@@ -1754,9 +1901,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>1</v>
+      </c>
       <c r="B94" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94">
         <v>111</v>
@@ -1768,9 +1918,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>1</v>
+      </c>
       <c r="B95" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C95">
         <v>134</v>
@@ -1782,9 +1935,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>1</v>
+      </c>
       <c r="B96" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C96">
         <v>135</v>
@@ -1796,9 +1952,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>1</v>
+      </c>
       <c r="B97" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C97">
         <v>136</v>
@@ -1810,9 +1969,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>1</v>
+      </c>
       <c r="B98" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C98">
         <v>140</v>
@@ -1824,12 +1986,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>1</v>
+      </c>
       <c r="B99" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C99" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D99">
         <v>98</v>
@@ -1838,9 +2003,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>1</v>
+      </c>
       <c r="B100" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C100">
         <v>159</v>
@@ -1852,9 +2020,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>1</v>
+      </c>
       <c r="B101" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C101">
         <v>160</v>
@@ -1866,9 +2037,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>1</v>
+      </c>
       <c r="B102" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C102">
         <v>161</v>
@@ -1880,9 +2054,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>1</v>
+      </c>
       <c r="B103" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C103">
         <v>162</v>
@@ -1894,12 +2071,15 @@
         <v>41</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>1</v>
+      </c>
       <c r="B104" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C104" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D104">
         <v>103</v>
@@ -1908,12 +2088,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>1</v>
+      </c>
       <c r="B105" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C105" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D105">
         <v>104</v>
@@ -1922,12 +2105,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>1</v>
+      </c>
       <c r="B106" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C106" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D106">
         <v>105</v>
@@ -1936,9 +2122,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>1</v>
+      </c>
       <c r="B107" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C107">
         <v>131</v>
@@ -1950,12 +2139,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>1</v>
+      </c>
       <c r="B108" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C108" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D108">
         <v>107</v>
@@ -1964,12 +2156,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>1</v>
+      </c>
       <c r="B109" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C109" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D109">
         <v>108</v>
@@ -1978,9 +2173,12 @@
         <v>47</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>1</v>
+      </c>
       <c r="B110" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C110">
         <v>174</v>
@@ -1992,9 +2190,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>1</v>
+      </c>
       <c r="B111" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C111">
         <v>184</v>
@@ -2006,9 +2207,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>1</v>
+      </c>
       <c r="B112" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C112">
         <v>201</v>
@@ -2020,9 +2224,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>1</v>
+      </c>
       <c r="B113" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C113">
         <v>209</v>
@@ -2034,9 +2241,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>1</v>
+      </c>
       <c r="B114" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C114">
         <v>212</v>
@@ -2048,9 +2258,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>1</v>
+      </c>
       <c r="B115" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C115">
         <v>214</v>
@@ -2062,9 +2275,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>1</v>
+      </c>
       <c r="B116" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C116">
         <v>239</v>
@@ -2076,9 +2292,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>1</v>
+      </c>
       <c r="B117" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C117">
         <v>240</v>
@@ -2090,9 +2309,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>1</v>
+      </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C118">
         <v>244</v>
@@ -2104,12 +2326,15 @@
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>1</v>
+      </c>
       <c r="B119" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C119" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D119">
         <v>118</v>
@@ -2118,9 +2343,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>1</v>
+      </c>
       <c r="B120" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C120">
         <v>20</v>
@@ -2132,12 +2360,15 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>1</v>
+      </c>
       <c r="B121" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C121" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D121">
         <v>120</v>
@@ -2146,12 +2377,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>1</v>
+      </c>
       <c r="B122" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C122" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D122">
         <v>121</v>
@@ -2160,12 +2394,15 @@
         <v>60</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>1</v>
+      </c>
       <c r="B123" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C123" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D123">
         <v>122</v>
@@ -2174,12 +2411,15 @@
         <v>61</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>1</v>
+      </c>
       <c r="B124" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C124" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D124">
         <v>123</v>
@@ -2188,12 +2428,15 @@
         <v>62</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>1</v>
+      </c>
       <c r="B125" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C125" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D125">
         <v>124</v>
@@ -2202,12 +2445,15 @@
         <v>63</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>1</v>
+      </c>
       <c r="B126" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C126" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D126">
         <v>125</v>
@@ -2216,9 +2462,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>1</v>
+      </c>
       <c r="B127" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C127">
         <v>1</v>
@@ -2230,9 +2479,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>1</v>
+      </c>
       <c r="B128" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C128">
         <v>2</v>
@@ -2244,9 +2496,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>1</v>
+      </c>
       <c r="B129" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C129">
         <v>3</v>
@@ -2258,9 +2513,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>1</v>
+      </c>
       <c r="B130" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C130">
         <v>4</v>
@@ -2272,12 +2530,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>1</v>
+      </c>
       <c r="B131" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C131" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D131">
         <v>130</v>
@@ -2286,9 +2547,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>1</v>
+      </c>
       <c r="B132" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C132">
         <v>9</v>
@@ -2300,12 +2564,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>1</v>
+      </c>
       <c r="B133" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C133" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D133">
         <v>132</v>
@@ -2314,12 +2581,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>1</v>
+      </c>
       <c r="B134" t="s">
-        <v>3</v>
-      </c>
-      <c r="C134" t="s">
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
       </c>
       <c r="D134">
         <v>133</v>
@@ -2328,9 +2598,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>1</v>
+      </c>
       <c r="B135" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C135">
         <v>11</v>
@@ -2342,12 +2615,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>1</v>
+      </c>
       <c r="B136" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C136" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D136">
         <v>135</v>
@@ -2356,9 +2632,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>1</v>
+      </c>
       <c r="B137" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C137">
         <v>15</v>
@@ -2370,9 +2649,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>1</v>
+      </c>
       <c r="B138" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C138">
         <v>23</v>
@@ -2384,12 +2666,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>1</v>
+      </c>
       <c r="B139" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C139" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D139">
         <v>138</v>
@@ -2398,12 +2683,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>1</v>
+      </c>
       <c r="B140" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C140" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D140">
         <v>139</v>
@@ -2412,9 +2700,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>1</v>
+      </c>
       <c r="B141" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C141">
         <v>41</v>
@@ -2425,13 +2716,19 @@
       <c r="E141" s="2">
         <v>15</v>
       </c>
-    </row>
-    <row r="142" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F141" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>1</v>
+      </c>
       <c r="B142" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C142" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D142">
         <v>141</v>
@@ -2440,12 +2737,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="143" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>1</v>
+      </c>
       <c r="B143" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C143" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D143">
         <v>142</v>
@@ -2453,13 +2753,19 @@
       <c r="E143" s="2">
         <v>17</v>
       </c>
-    </row>
-    <row r="144" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="F143" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>1</v>
+      </c>
       <c r="B144" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C144" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D144">
         <v>143</v>
@@ -2467,13 +2773,19 @@
       <c r="E144" s="2">
         <v>18</v>
       </c>
-    </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F144" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>1</v>
+      </c>
       <c r="B145" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C145" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D145">
         <v>144</v>
@@ -2481,13 +2793,19 @@
       <c r="E145" s="2">
         <v>19</v>
       </c>
-    </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F145" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>1</v>
+      </c>
       <c r="B146" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C146" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D146">
         <v>145</v>
@@ -2495,13 +2813,19 @@
       <c r="E146" s="2">
         <v>20</v>
       </c>
-    </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F146" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>1</v>
+      </c>
       <c r="B147" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C147" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D147">
         <v>146</v>
@@ -2509,10 +2833,16 @@
       <c r="E147" s="2">
         <v>21</v>
       </c>
-    </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="F147" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>1</v>
+      </c>
       <c r="B148" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C148">
         <v>55</v>
@@ -2524,9 +2854,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>1</v>
+      </c>
       <c r="B149" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C149">
         <v>56</v>
@@ -2538,9 +2871,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>1</v>
+      </c>
       <c r="B150" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C150">
         <v>57</v>
@@ -2552,9 +2888,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>1</v>
+      </c>
       <c r="B151" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C151">
         <v>58</v>
@@ -2566,9 +2905,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>1</v>
+      </c>
       <c r="B152" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C152">
         <v>59</v>
@@ -2580,9 +2922,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>1</v>
+      </c>
       <c r="B153" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C153">
         <v>60</v>
@@ -2594,9 +2939,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>1</v>
+      </c>
       <c r="B154" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C154">
         <v>61</v>
@@ -2608,9 +2956,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>1</v>
+      </c>
       <c r="B155" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C155">
         <v>62</v>
@@ -2622,12 +2973,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>1</v>
+      </c>
       <c r="B156" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C156" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D156">
         <v>155</v>
@@ -2640,7 +2994,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>1</v>
+      </c>
       <c r="C157">
         <v>66</v>
       </c>
@@ -2651,9 +3008,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>1</v>
+      </c>
       <c r="C158" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D158">
         <v>157</v>
@@ -2662,7 +3022,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>1</v>
+      </c>
       <c r="C159">
         <v>73</v>
       </c>
@@ -2673,7 +3036,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>1</v>
+      </c>
       <c r="C160">
         <v>80</v>
       </c>
@@ -2684,7 +3050,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>1</v>
+      </c>
       <c r="C161">
         <v>100</v>
       </c>
@@ -2695,9 +3064,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="162" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>1</v>
+      </c>
       <c r="C162" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D162">
         <v>161</v>
@@ -2706,8 +3078,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="163" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C163">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>1</v>
+      </c>
+      <c r="C163" s="3">
         <v>108</v>
       </c>
       <c r="D163">
@@ -2716,9 +3091,15 @@
       <c r="E163" s="2">
         <v>7</v>
       </c>
-    </row>
-    <row r="164" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C164">
+      <c r="F163" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>1</v>
+      </c>
+      <c r="C164" s="3">
         <v>109</v>
       </c>
       <c r="D164">
@@ -2728,8 +3109,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="165" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C165">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>1</v>
+      </c>
+      <c r="C165" s="3">
         <v>120</v>
       </c>
       <c r="D165">
@@ -2739,7 +3123,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>1</v>
+      </c>
       <c r="C166">
         <v>123</v>
       </c>
@@ -2750,9 +3137,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="167" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>1</v>
+      </c>
       <c r="C167" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D167">
         <v>166</v>
@@ -2761,7 +3151,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="168" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>1</v>
+      </c>
       <c r="C168">
         <v>172</v>
       </c>
@@ -2772,7 +3165,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C169">
         <v>182</v>
       </c>
@@ -2782,10 +3175,13 @@
       <c r="E169" s="2">
         <v>13</v>
       </c>
-    </row>
-    <row r="170" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="F169" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C170" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D170">
         <v>169</v>
@@ -2793,8 +3189,14 @@
       <c r="E170" s="2">
         <v>14</v>
       </c>
-    </row>
-    <row r="171" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="F170" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>1</v>
+      </c>
       <c r="C171">
         <v>200</v>
       </c>
@@ -2805,7 +3207,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="172" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>1</v>
+      </c>
       <c r="C172">
         <v>243</v>
       </c>
@@ -2818,5 +3223,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>